<commit_message>
ETRS & Schedule Notify
</commit_message>
<xml_diff>
--- a/testData/ExecuteTask/Notification/ETRS/ET_NT_ETRS_DTBeforeMinutes_Test.xlsx
+++ b/testData/ExecuteTask/Notification/ETRS/ET_NT_ETRS_DTBeforeMinutes_Test.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="107">
   <si>
     <t>ModuleName</t>
   </si>
@@ -316,6 +316,33 @@
   </si>
   <si>
     <t>08:00:00 PM</t>
+  </si>
+  <si>
+    <t>28-05-2024</t>
+  </si>
+  <si>
+    <t>31-05-2024 05:00:00 PM</t>
+  </si>
+  <si>
+    <t>ET416</t>
+  </si>
+  <si>
+    <t>31-05-2024 06:00:00 PM</t>
+  </si>
+  <si>
+    <t>06:00:00 AM</t>
+  </si>
+  <si>
+    <t>31-05-2024 07:00:00 PM</t>
+  </si>
+  <si>
+    <t>07:00:00 AM</t>
+  </si>
+  <si>
+    <t>31-05-2024 08:00:00 PM</t>
+  </si>
+  <si>
+    <t>08:00:00 AM</t>
   </si>
 </sst>
 </file>
@@ -861,7 +888,7 @@
         <v>31</v>
       </c>
       <c r="K2" t="s" s="1">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="L2" s="1">
         <v>1</v>
@@ -870,10 +897,10 @@
         <v>32</v>
       </c>
       <c r="N2" t="s" s="1">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="O2" t="s" s="1">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>33</v>
@@ -921,7 +948,7 @@
         <v>82</v>
       </c>
       <c r="AG2" t="s" s="1">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="AH2" s="7">
         <v>5</v>
@@ -1117,7 +1144,7 @@
         <v>31</v>
       </c>
       <c r="K2" t="s" s="0">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="L2" s="1">
         <v>1</v>
@@ -1126,10 +1153,10 @@
         <v>32</v>
       </c>
       <c r="N2" t="s" s="0">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="O2" t="s" s="0">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>33</v>
@@ -1362,7 +1389,7 @@
         <v>31</v>
       </c>
       <c r="K2" t="s" s="0">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="L2" s="1">
         <v>1</v>
@@ -1371,10 +1398,10 @@
         <v>32</v>
       </c>
       <c r="N2" t="s" s="0">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="O2" t="s" s="0">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>33</v>
@@ -1638,7 +1665,7 @@
         <v>31</v>
       </c>
       <c r="K2" t="s" s="0">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="L2" s="1">
         <v>1</v>
@@ -1647,10 +1674,10 @@
         <v>32</v>
       </c>
       <c r="N2" t="s" s="0">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="O2" t="s" s="0">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>33</v>

</xml_diff>